<commit_message>
Added a mesh creator and created a rudimentary random terrain maker.
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CDDA2D-75B4-4644-A72E-589E0E6EB862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01A1E96-9FA2-4279-A404-2284E50C3A56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>Student Git Address:  https://github.com/MyNameIsJeffery/VoidGraphics</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -930,7 +936,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,15 +1050,19 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G67" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 18, 18, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 18, 18, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1064,11 +1074,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1125,7 +1135,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 18, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 18,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 18, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 18,0)</f>
@@ -1154,11 +1164,15 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>22</v>
@@ -1193,7 +1207,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -1498,11 +1512,15 @@
       <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1659,11 +1677,15 @@
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
+      <c r="E28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -1862,11 +1884,15 @@
       <c r="D37" s="5">
         <v>1</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="3"/>
+      <c r="E37" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G37" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -1887,11 +1913,15 @@
       <c r="D38" s="5">
         <v>1</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G38" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -3063,7 +3093,9 @@
       <c r="B91" s="6">
         <v>2</v>
       </c>
-      <c r="C91" s="3"/>
+      <c r="C91" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
@@ -3216,7 +3248,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added the ability to take obj headers and turn them into objs. With this I was able to correctly test my normal shader.
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01A1E96-9FA2-4279-A404-2284E50C3A56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81BB32A-915E-452E-B7FF-B20BF5F68C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -936,7 +936,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 18, 18, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 18, 18, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1074,11 +1074,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 18, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 18,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 18, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 18,0)</f>
@@ -1167,12 +1167,10 @@
       <c r="E7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>22</v>
@@ -1207,7 +1205,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -1515,12 +1513,10 @@
       <c r="E21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1680,12 +1676,10 @@
       <c r="E28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="F28" s="3"/>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -3248,7 +3242,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Went with STB since I didn't get a response from lari, and the KTX converter kept crashing.
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81BB32A-915E-452E-B7FF-B20BF5F68C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7575EC-811C-4C0B-8940-7F3A21F199D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -936,7 +936,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 18, 18, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 18, 18, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -1513,10 +1513,12 @@
       <c r="E21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1676,10 +1678,12 @@
       <c r="E28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -3242,7 +3246,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Replaced STB with FTX support.
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7575EC-811C-4C0B-8940-7F3A21F199D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932D45EC-DCDB-48DE-ADD1-20C0FE0FEBB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -935,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3246,7 +3246,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Renamed files to better understand what they are. Fixed issue with directional light not being a directional light.
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932D45EC-DCDB-48DE-ADD1-20C0FE0FEBB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843A0543-24BE-4CDC-BD31-66B6C92977C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -935,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,11 +1074,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 18, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 18,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 18, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 18,0)</f>
@@ -1164,9 +1164,7 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="3"/>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
@@ -1197,11 +1195,15 @@
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>

</xml_diff>

<commit_message>
updated lights to be easier to control. Added point lights and combined them with directional lights. Both of which can be updated each frame.
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843A0543-24BE-4CDC-BD31-66B6C92977C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E289D01E-35BB-4909-A162-336232D26138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -936,7 +939,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1069,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 18, 18, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 18, 18, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1074,11 +1077,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>19</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1094,11 +1097,15 @@
       <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>26</v>
@@ -1139,7 +1146,7 @@
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 18, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 18,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 18, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 18,0)</f>
@@ -1164,11 +1171,15 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>22</v>
@@ -1211,11 +1222,11 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1233,11 +1244,15 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>25</v>
@@ -1272,11 +1287,11 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -1731,11 +1746,15 @@
       <c r="D30" s="5">
         <v>2</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1967,11 +1986,15 @@
       <c r="D40" s="5">
         <v>3</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G40" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -1992,11 +2015,15 @@
       <c r="D41" s="5">
         <v>3</v>
       </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="3"/>
+      <c r="E41" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G41" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -2117,11 +2144,15 @@
       <c r="D46" s="5">
         <v>2</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="3"/>
+      <c r="E46" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G46" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -3096,7 +3127,9 @@
       <c r="C91" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -3248,7 +3281,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added reflective materials. cleaned up errors.
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E289D01E-35BB-4909-A162-336232D26138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD21BA5-3243-463D-B764-D6B5C3AE1EC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5550" yWindow="825" windowWidth="14220" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="109">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -345,6 +345,18 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>https://www.glfw.org/</t>
+  </si>
+  <si>
+    <t>https://glad.dav1d.de/</t>
+  </si>
+  <si>
+    <t>https://www.khronos.org/ktx/documentation/libktx/index.html</t>
+  </si>
+  <si>
+    <t>https://glm.g-truc.net/0.9.9/index.html</t>
   </si>
 </sst>
 </file>
@@ -938,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3191,16 +3203,24 @@
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" s="12"/>
+      <c r="A96" s="12" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="12"/>
+      <c r="A97" s="12" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="12"/>
+      <c r="A98" s="12" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
+      <c r="A99" s="12" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
@@ -3281,7 +3301,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added camera controls and README.txt.
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD21BA5-3243-463D-B764-D6B5C3AE1EC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AD6CCF-1646-4833-B60A-2245CC9748F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="825" windowWidth="14220" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="110">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>https://glm.g-truc.net/0.9.9/index.html</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -950,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1088,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 18, 18, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1093,7 +1096,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1167,7 +1170,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1238,7 +1241,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1350,11 +1353,15 @@
       <c r="D12" s="5">
         <v>4</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G12" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1425,11 +1432,15 @@
       <c r="D15" s="5">
         <v>2</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
+      <c r="E15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1618,11 +1629,15 @@
       <c r="D24" s="5">
         <v>3</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G24" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1733,11 +1748,15 @@
       <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
+      <c r="E29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G29" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1787,11 +1806,15 @@
       <c r="D31" s="5">
         <v>4</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G31" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -2399,7 +2422,9 @@
       <c r="D57" s="5">
         <v>2</v>
       </c>
-      <c r="E57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="F57" s="3"/>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
@@ -2527,7 +2552,9 @@
       <c r="D63" s="5">
         <v>2</v>
       </c>
-      <c r="E63" s="2"/>
+      <c r="E63" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="F63" s="3"/>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
@@ -2652,7 +2679,9 @@
       <c r="D68" s="5">
         <v>4</v>
       </c>
-      <c r="E68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="F68" s="3"/>
       <c r="G68" s="16">
         <f t="shared" ref="G68:G89" si="1" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
@@ -2730,7 +2759,9 @@
       <c r="D72" s="5">
         <v>2</v>
       </c>
-      <c r="E72" s="2"/>
+      <c r="E72" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="F72" s="3"/>
       <c r="G72" s="16">
         <f t="shared" si="1"/>
@@ -2954,7 +2985,9 @@
       <c r="D82" s="5">
         <v>3</v>
       </c>
-      <c r="E82" s="2"/>
+      <c r="E82" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="F82" s="3"/>
       <c r="G82" s="16">
         <f t="shared" si="1"/>
@@ -3301,7 +3334,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added shader controls. Added final objects. Added fullscreen effects.(grayscale)
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D566D1D-DBB6-495D-8CE6-44F24268ED06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429A5F2F-C4ED-41F0-8B52-4898DA2A9035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="825" windowWidth="14220" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="115">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,12 +1371,10 @@
       <c r="E12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="F12" s="3"/>
       <c r="G12" s="16">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1766,12 +1764,10 @@
       <c r="E29" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="F29" s="3"/>
       <c r="G29" s="16">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1824,12 +1820,10 @@
       <c r="E31" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="F31" s="3"/>
       <c r="G31" s="16">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -2440,10 +2434,12 @@
       <c r="E57" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F57" s="3"/>
+      <c r="F57" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2570,10 +2566,12 @@
       <c r="E63" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F63" s="3"/>
+      <c r="F63" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
@@ -2777,10 +2775,12 @@
       <c r="E72" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F72" s="3"/>
+      <c r="F72" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G72" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
@@ -3003,10 +3003,12 @@
       <c r="E82" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F82" s="3"/>
+      <c r="F82" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G82" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>

</xml_diff>

<commit_message>
Final push. Added secondary scene with knight and flag. I wish I could have done more.
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429A5F2F-C4ED-41F0-8B52-4898DA2A9035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFA3148-6974-4CD6-BD1C-533DFDB95A53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="115">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,15 +1103,15 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 18, 18, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1180,12 +1180,12 @@
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 18, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 18,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1317,15 +1317,15 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1368,9 +1368,7 @@
       <c r="D12" s="5">
         <v>4</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="3"/>
       <c r="G12" s="16">
         <f t="shared" si="0"/>
@@ -1761,9 +1759,7 @@
       <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="E29" s="2"/>
       <c r="F29" s="3"/>
       <c r="G29" s="16">
         <f t="shared" si="0"/>
@@ -1817,9 +1813,7 @@
       <c r="D31" s="5">
         <v>4</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="E31" s="2"/>
       <c r="F31" s="3"/>
       <c r="G31" s="16">
         <f t="shared" si="0"/>
@@ -2692,9 +2686,7 @@
       <c r="D68" s="5">
         <v>4</v>
       </c>
-      <c r="E68" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="E68" s="2"/>
       <c r="F68" s="3"/>
       <c r="G68" s="16">
         <f t="shared" ref="G68:G89" si="1" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
@@ -3025,11 +3017,15 @@
       <c r="D83" s="5">
         <v>4</v>
       </c>
-      <c r="E83" s="2"/>
-      <c r="F83" s="3"/>
+      <c r="E83" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G83" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
@@ -3192,7 +3188,9 @@
       <c r="D91" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3361,7 +3359,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>